<commit_message>
Update in the dataset
</commit_message>
<xml_diff>
--- a/Supervised ML/Train_Test_Split/mpg.xlsx
+++ b/Supervised ML/Train_Test_Split/mpg.xlsx
@@ -1,27 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\ML\ch1_supervised_learning_regression\4_train_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitudru\Documents\step-into-ml\Supervised ML\Train_Test_Split\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAAB3A5B-C4E7-462C-BDDB-8A8E79207D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEAC388-4596-4C4D-A797-5E3428FBBE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="39540" yWindow="1005" windowWidth="19200" windowHeight="10515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mpg" sheetId="1" r:id="rId1"/>
-    <sheet name="r_squared_score_calculation" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="315">
   <si>
     <t>mpg</t>
   </si>
@@ -966,42 +976,12 @@
   </si>
   <si>
     <t>chevy s-10</t>
-  </si>
-  <si>
-    <t>Truth</t>
-  </si>
-  <si>
-    <t>SST</t>
-  </si>
-  <si>
-    <t>SSR</t>
-  </si>
-  <si>
-    <t>diff</t>
-  </si>
-  <si>
-    <t>diff**2</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>Prediction 2</t>
-  </si>
-  <si>
-    <t>Prediction 1</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>R**2 Score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1138,7 +1118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1330,12 +1310,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1497,15 +1471,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1553,7 +1523,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1882,28 +1852,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I399"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" customWidth="1"/>
+    <col min="4" max="4" width="7.54296875" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
     <col min="8" max="8" width="27" customWidth="1"/>
-    <col min="9" max="9" width="5.140625" customWidth="1"/>
+    <col min="9" max="9" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1932,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>8</v>
       </c>
@@ -1961,7 +1931,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>8</v>
       </c>
@@ -1990,7 +1960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>8</v>
       </c>
@@ -2019,7 +1989,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>8</v>
       </c>
@@ -2048,7 +2018,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>8</v>
       </c>
@@ -2077,7 +2047,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>8</v>
       </c>
@@ -2106,7 +2076,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2135,7 +2105,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2164,7 +2134,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2193,7 +2163,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2222,7 +2192,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2251,7 +2221,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>8</v>
       </c>
@@ -2280,7 +2250,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>8</v>
       </c>
@@ -2309,7 +2279,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>8</v>
       </c>
@@ -2338,7 +2308,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>4</v>
       </c>
@@ -2367,7 +2337,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>6</v>
       </c>
@@ -2396,7 +2366,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>6</v>
       </c>
@@ -2425,7 +2395,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>6</v>
       </c>
@@ -2454,7 +2424,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>4</v>
       </c>
@@ -2483,7 +2453,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2512,7 +2482,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>4</v>
       </c>
@@ -2541,7 +2511,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>4</v>
       </c>
@@ -2570,7 +2540,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>4</v>
       </c>
@@ -2599,7 +2569,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>4</v>
       </c>
@@ -2628,7 +2598,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>6</v>
       </c>
@@ -2657,7 +2627,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>8</v>
       </c>
@@ -2686,7 +2656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>8</v>
       </c>
@@ -2715,7 +2685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>8</v>
       </c>
@@ -2744,7 +2714,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>8</v>
       </c>
@@ -2773,7 +2743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2802,7 +2772,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2831,7 +2801,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2860,7 +2830,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2889,7 +2859,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>6</v>
       </c>
@@ -2918,7 +2888,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>6</v>
       </c>
@@ -2947,7 +2917,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>6</v>
       </c>
@@ -2976,7 +2946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>6</v>
       </c>
@@ -3005,7 +2975,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>6</v>
       </c>
@@ -3034,7 +3004,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>8</v>
       </c>
@@ -3063,7 +3033,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>8</v>
       </c>
@@ -3092,7 +3062,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>8</v>
       </c>
@@ -3121,7 +3091,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>8</v>
       </c>
@@ -3150,7 +3120,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>8</v>
       </c>
@@ -3179,7 +3149,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>8</v>
       </c>
@@ -3208,7 +3178,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>8</v>
       </c>
@@ -3237,7 +3207,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>6</v>
       </c>
@@ -3266,7 +3236,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>4</v>
       </c>
@@ -3295,7 +3265,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>6</v>
       </c>
@@ -3324,7 +3294,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>6</v>
       </c>
@@ -3353,7 +3323,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>4</v>
       </c>
@@ -3382,7 +3352,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>4</v>
       </c>
@@ -3411,7 +3381,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>4</v>
       </c>
@@ -3440,7 +3410,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>4</v>
       </c>
@@ -3469,7 +3439,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>4</v>
       </c>
@@ -3498,7 +3468,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>4</v>
       </c>
@@ -3527,7 +3497,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>4</v>
       </c>
@@ -3556,7 +3526,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>4</v>
       </c>
@@ -3585,7 +3555,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>4</v>
       </c>
@@ -3614,7 +3584,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>4</v>
       </c>
@@ -3643,7 +3613,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>4</v>
       </c>
@@ -3672,7 +3642,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>4</v>
       </c>
@@ -3701,7 +3671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>4</v>
       </c>
@@ -3730,7 +3700,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>8</v>
       </c>
@@ -3759,7 +3729,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>8</v>
       </c>
@@ -3788,7 +3758,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>8</v>
       </c>
@@ -3817,7 +3787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>8</v>
       </c>
@@ -3846,7 +3816,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>8</v>
       </c>
@@ -3875,7 +3845,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>8</v>
       </c>
@@ -3904,7 +3874,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>8</v>
       </c>
@@ -3933,7 +3903,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>8</v>
       </c>
@@ -3962,7 +3932,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>8</v>
       </c>
@@ -3991,7 +3961,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>3</v>
       </c>
@@ -4020,7 +3990,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>8</v>
       </c>
@@ -4049,7 +4019,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>8</v>
       </c>
@@ -4078,7 +4048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>8</v>
       </c>
@@ -4107,7 +4077,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>8</v>
       </c>
@@ -4136,7 +4106,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>4</v>
       </c>
@@ -4165,7 +4135,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>4</v>
       </c>
@@ -4194,7 +4164,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>4</v>
       </c>
@@ -4223,7 +4193,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>4</v>
       </c>
@@ -4252,7 +4222,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>4</v>
       </c>
@@ -4281,7 +4251,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>4</v>
       </c>
@@ -4310,7 +4280,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>4</v>
       </c>
@@ -4339,7 +4309,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>4</v>
       </c>
@@ -4368,7 +4338,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>4</v>
       </c>
@@ -4397,7 +4367,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>8</v>
       </c>
@@ -4426,7 +4396,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>8</v>
       </c>
@@ -4455,7 +4425,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>8</v>
       </c>
@@ -4484,7 +4454,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>8</v>
       </c>
@@ -4513,7 +4483,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>8</v>
       </c>
@@ -4542,7 +4512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>8</v>
       </c>
@@ -4571,7 +4541,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>8</v>
       </c>
@@ -4600,7 +4570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>8</v>
       </c>
@@ -4629,7 +4599,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>8</v>
       </c>
@@ -4658,7 +4628,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>8</v>
       </c>
@@ -4687,7 +4657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>8</v>
       </c>
@@ -4716,7 +4686,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>8</v>
       </c>
@@ -4745,7 +4715,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>6</v>
       </c>
@@ -4774,7 +4744,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>6</v>
       </c>
@@ -4803,7 +4773,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>6</v>
       </c>
@@ -4832,7 +4802,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>6</v>
       </c>
@@ -4861,7 +4831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>6</v>
       </c>
@@ -4890,7 +4860,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>4</v>
       </c>
@@ -4919,7 +4889,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>8</v>
       </c>
@@ -4948,7 +4918,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>8</v>
       </c>
@@ -4977,7 +4947,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>8</v>
       </c>
@@ -5006,7 +4976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>8</v>
       </c>
@@ -5035,7 +5005,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>6</v>
       </c>
@@ -5064,7 +5034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>4</v>
       </c>
@@ -5093,7 +5063,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>4</v>
       </c>
@@ -5122,7 +5092,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>4</v>
       </c>
@@ -5151,7 +5121,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>3</v>
       </c>
@@ -5180,7 +5150,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>4</v>
       </c>
@@ -5209,7 +5179,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>6</v>
       </c>
@@ -5238,7 +5208,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>4</v>
       </c>
@@ -5267,7 +5237,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>8</v>
       </c>
@@ -5296,7 +5266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>8</v>
       </c>
@@ -5325,7 +5295,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>4</v>
       </c>
@@ -5354,7 +5324,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>4</v>
       </c>
@@ -5383,7 +5353,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>4</v>
       </c>
@@ -5412,7 +5382,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>4</v>
       </c>
@@ -5441,7 +5411,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>8</v>
       </c>
@@ -5470,7 +5440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>4</v>
       </c>
@@ -5499,7 +5469,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>6</v>
       </c>
@@ -5528,7 +5498,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>8</v>
       </c>
@@ -5557,7 +5527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>6</v>
       </c>
@@ -5586,7 +5556,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>6</v>
       </c>
@@ -5615,7 +5585,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>6</v>
       </c>
@@ -5644,7 +5614,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>6</v>
       </c>
@@ -5673,7 +5643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>4</v>
       </c>
@@ -5702,7 +5672,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>4</v>
       </c>
@@ -5731,7 +5701,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>4</v>
       </c>
@@ -5760,7 +5730,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>4</v>
       </c>
@@ -5789,7 +5759,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>6</v>
       </c>
@@ -5818,7 +5788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>6</v>
       </c>
@@ -5847,7 +5817,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>6</v>
       </c>
@@ -5876,7 +5846,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>8</v>
       </c>
@@ -5905,7 +5875,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>8</v>
       </c>
@@ -5934,7 +5904,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>8</v>
       </c>
@@ -5963,7 +5933,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>8</v>
       </c>
@@ -5992,7 +5962,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>8</v>
       </c>
@@ -6021,7 +5991,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>4</v>
       </c>
@@ -6050,7 +6020,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>4</v>
       </c>
@@ -6079,7 +6049,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>4</v>
       </c>
@@ -6108,7 +6078,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>4</v>
       </c>
@@ -6137,7 +6107,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>4</v>
       </c>
@@ -6166,7 +6136,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>4</v>
       </c>
@@ -6195,7 +6165,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>4</v>
       </c>
@@ -6224,7 +6194,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>4</v>
       </c>
@@ -6253,7 +6223,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>4</v>
       </c>
@@ -6282,7 +6252,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>4</v>
       </c>
@@ -6311,7 +6281,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>4</v>
       </c>
@@ -6340,7 +6310,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>6</v>
       </c>
@@ -6369,7 +6339,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>6</v>
       </c>
@@ -6398,7 +6368,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>6</v>
       </c>
@@ -6427,7 +6397,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>6</v>
       </c>
@@ -6456,7 +6426,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>8</v>
       </c>
@@ -6485,7 +6455,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>8</v>
       </c>
@@ -6514,7 +6484,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>8</v>
       </c>
@@ -6543,7 +6513,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>8</v>
       </c>
@@ -6572,7 +6542,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>6</v>
       </c>
@@ -6601,7 +6571,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>6</v>
       </c>
@@ -6630,7 +6600,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>6</v>
       </c>
@@ -6659,7 +6629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>6</v>
       </c>
@@ -6688,7 +6658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>6</v>
       </c>
@@ -6717,7 +6687,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>8</v>
       </c>
@@ -6746,7 +6716,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>8</v>
       </c>
@@ -6775,7 +6745,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>4</v>
       </c>
@@ -6804,7 +6774,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>4</v>
       </c>
@@ -6833,7 +6803,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>6</v>
       </c>
@@ -6862,7 +6832,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>4</v>
       </c>
@@ -6891,7 +6861,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>4</v>
       </c>
@@ -6920,7 +6890,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>4</v>
       </c>
@@ -6949,7 +6919,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>4</v>
       </c>
@@ -6978,7 +6948,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>6</v>
       </c>
@@ -7007,7 +6977,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>4</v>
       </c>
@@ -7036,7 +7006,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>6</v>
       </c>
@@ -7065,7 +7035,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>4</v>
       </c>
@@ -7094,7 +7064,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>4</v>
       </c>
@@ -7123,7 +7093,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>4</v>
       </c>
@@ -7152,7 +7122,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>4</v>
       </c>
@@ -7181,7 +7151,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>4</v>
       </c>
@@ -7210,7 +7180,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>4</v>
       </c>
@@ -7239,7 +7209,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>4</v>
       </c>
@@ -7268,7 +7238,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>4</v>
       </c>
@@ -7297,7 +7267,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>4</v>
       </c>
@@ -7326,7 +7296,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>4</v>
       </c>
@@ -7355,7 +7325,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>8</v>
       </c>
@@ -7384,7 +7354,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>8</v>
       </c>
@@ -7413,7 +7383,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>8</v>
       </c>
@@ -7442,7 +7412,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>8</v>
       </c>
@@ -7471,7 +7441,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>6</v>
       </c>
@@ -7500,7 +7470,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>6</v>
       </c>
@@ -7529,7 +7499,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>6</v>
       </c>
@@ -7558,7 +7528,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>6</v>
       </c>
@@ -7587,7 +7557,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>4</v>
       </c>
@@ -7616,7 +7586,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>4</v>
       </c>
@@ -7645,7 +7615,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>4</v>
       </c>
@@ -7674,7 +7644,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>4</v>
       </c>
@@ -7703,7 +7673,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>6</v>
       </c>
@@ -7732,7 +7702,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>6</v>
       </c>
@@ -7761,7 +7731,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>6</v>
       </c>
@@ -7790,7 +7760,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>6</v>
       </c>
@@ -7819,7 +7789,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>4</v>
       </c>
@@ -7848,7 +7818,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>4</v>
       </c>
@@ -7877,7 +7847,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>4</v>
       </c>
@@ -7906,7 +7876,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>4</v>
       </c>
@@ -7935,7 +7905,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>4</v>
       </c>
@@ -7964,7 +7934,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>8</v>
       </c>
@@ -7993,7 +7963,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>4</v>
       </c>
@@ -8022,7 +7992,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>6</v>
       </c>
@@ -8051,7 +8021,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>6</v>
       </c>
@@ -8080,7 +8050,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>8</v>
       </c>
@@ -8109,7 +8079,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>8</v>
       </c>
@@ -8138,7 +8108,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>8</v>
       </c>
@@ -8167,7 +8137,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>8</v>
       </c>
@@ -8196,7 +8166,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>4</v>
       </c>
@@ -8225,7 +8195,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>4</v>
       </c>
@@ -8254,7 +8224,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>4</v>
       </c>
@@ -8283,7 +8253,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>4</v>
       </c>
@@ -8312,7 +8282,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>4</v>
       </c>
@@ -8341,7 +8311,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>8</v>
       </c>
@@ -8370,7 +8340,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>8</v>
       </c>
@@ -8399,7 +8369,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>8</v>
       </c>
@@ -8428,7 +8398,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>8</v>
       </c>
@@ -8457,7 +8427,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>6</v>
       </c>
@@ -8486,7 +8456,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>6</v>
       </c>
@@ -8515,7 +8485,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>6</v>
       </c>
@@ -8544,7 +8514,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>6</v>
       </c>
@@ -8573,7 +8543,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>8</v>
       </c>
@@ -8602,7 +8572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>8</v>
       </c>
@@ -8631,7 +8601,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>8</v>
       </c>
@@ -8660,7 +8630,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>8</v>
       </c>
@@ -8689,7 +8659,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>4</v>
       </c>
@@ -8718,7 +8688,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>4</v>
       </c>
@@ -8747,7 +8717,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>4</v>
       </c>
@@ -8776,7 +8746,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>4</v>
       </c>
@@ -8805,7 +8775,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>4</v>
       </c>
@@ -8834,7 +8804,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>4</v>
       </c>
@@ -8863,7 +8833,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>4</v>
       </c>
@@ -8892,7 +8862,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>4</v>
       </c>
@@ -8921,7 +8891,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>6</v>
       </c>
@@ -8950,7 +8920,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>4</v>
       </c>
@@ -8979,7 +8949,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>3</v>
       </c>
@@ -9008,7 +8978,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>4</v>
       </c>
@@ -9037,7 +9007,7 @@
         <v>43.1</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>4</v>
       </c>
@@ -9066,7 +9036,7 @@
         <v>36.1</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>4</v>
       </c>
@@ -9095,7 +9065,7 @@
         <v>32.799999999999997</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>4</v>
       </c>
@@ -9124,7 +9094,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>4</v>
       </c>
@@ -9153,7 +9123,7 @@
         <v>36.1</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>8</v>
       </c>
@@ -9182,7 +9152,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>8</v>
       </c>
@@ -9211,7 +9181,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>8</v>
       </c>
@@ -9240,7 +9210,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A254">
         <v>6</v>
       </c>
@@ -9269,7 +9239,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A255">
         <v>6</v>
       </c>
@@ -9298,7 +9268,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A256">
         <v>6</v>
       </c>
@@ -9327,7 +9297,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A257">
         <v>4</v>
       </c>
@@ -9356,7 +9326,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A258">
         <v>6</v>
       </c>
@@ -9385,7 +9355,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A259">
         <v>6</v>
       </c>
@@ -9414,7 +9384,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A260">
         <v>6</v>
       </c>
@@ -9443,7 +9413,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A261">
         <v>6</v>
       </c>
@@ -9472,7 +9442,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A262">
         <v>6</v>
       </c>
@@ -9501,7 +9471,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A263">
         <v>6</v>
       </c>
@@ -9530,7 +9500,7 @@
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A264">
         <v>8</v>
       </c>
@@ -9559,7 +9529,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A265">
         <v>6</v>
       </c>
@@ -9588,7 +9558,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A266">
         <v>8</v>
       </c>
@@ -9617,7 +9587,7 @@
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A267">
         <v>8</v>
       </c>
@@ -9646,7 +9616,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A268">
         <v>4</v>
       </c>
@@ -9675,7 +9645,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A269">
         <v>4</v>
       </c>
@@ -9704,7 +9674,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A270">
         <v>4</v>
       </c>
@@ -9733,7 +9703,7 @@
         <v>27.2</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A271">
         <v>4</v>
       </c>
@@ -9762,7 +9732,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A272">
         <v>4</v>
       </c>
@@ -9791,7 +9761,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A273">
         <v>4</v>
       </c>
@@ -9820,7 +9790,7 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A274">
         <v>4</v>
       </c>
@@ -9849,7 +9819,7 @@
         <v>23.8</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A275">
         <v>4</v>
       </c>
@@ -9878,7 +9848,7 @@
         <v>23.9</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A276">
         <v>5</v>
       </c>
@@ -9907,7 +9877,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A277">
         <v>6</v>
       </c>
@@ -9936,7 +9906,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A278">
         <v>4</v>
       </c>
@@ -9965,7 +9935,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A279">
         <v>6</v>
       </c>
@@ -9994,7 +9964,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A280">
         <v>4</v>
       </c>
@@ -10023,7 +9993,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A281">
         <v>4</v>
       </c>
@@ -10052,7 +10022,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A282">
         <v>6</v>
       </c>
@@ -10081,7 +10051,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A283">
         <v>6</v>
       </c>
@@ -10110,7 +10080,7 @@
         <v>19.8</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A284">
         <v>4</v>
       </c>
@@ -10139,7 +10109,7 @@
         <v>22.3</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A285">
         <v>6</v>
       </c>
@@ -10168,7 +10138,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A286">
         <v>6</v>
       </c>
@@ -10197,7 +10167,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A287">
         <v>8</v>
       </c>
@@ -10226,7 +10196,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A288">
         <v>8</v>
       </c>
@@ -10255,7 +10225,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A289">
         <v>8</v>
       </c>
@@ -10284,7 +10254,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A290">
         <v>8</v>
       </c>
@@ -10313,7 +10283,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A291">
         <v>8</v>
       </c>
@@ -10342,7 +10312,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A292">
         <v>8</v>
       </c>
@@ -10371,7 +10341,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A293">
         <v>8</v>
       </c>
@@ -10400,7 +10370,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A294">
         <v>8</v>
       </c>
@@ -10429,7 +10399,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A295">
         <v>4</v>
       </c>
@@ -10458,7 +10428,7 @@
         <v>31.9</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A296">
         <v>4</v>
       </c>
@@ -10487,7 +10457,7 @@
         <v>34.1</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A297">
         <v>4</v>
       </c>
@@ -10516,7 +10486,7 @@
         <v>35.700000000000003</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A298">
         <v>4</v>
       </c>
@@ -10545,7 +10515,7 @@
         <v>27.4</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A299">
         <v>5</v>
       </c>
@@ -10574,7 +10544,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A300">
         <v>8</v>
       </c>
@@ -10603,7 +10573,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A301">
         <v>4</v>
       </c>
@@ -10632,7 +10602,7 @@
         <v>27.2</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A302">
         <v>8</v>
       </c>
@@ -10661,7 +10631,7 @@
         <v>23.9</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A303">
         <v>4</v>
       </c>
@@ -10690,7 +10660,7 @@
         <v>34.200000000000003</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A304">
         <v>4</v>
       </c>
@@ -10719,7 +10689,7 @@
         <v>34.5</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A305">
         <v>4</v>
       </c>
@@ -10748,7 +10718,7 @@
         <v>31.8</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A306">
         <v>4</v>
       </c>
@@ -10777,7 +10747,7 @@
         <v>37.299999999999997</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A307">
         <v>4</v>
       </c>
@@ -10806,7 +10776,7 @@
         <v>28.4</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A308">
         <v>6</v>
       </c>
@@ -10835,7 +10805,7 @@
         <v>28.8</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A309">
         <v>6</v>
       </c>
@@ -10864,7 +10834,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A310">
         <v>4</v>
       </c>
@@ -10893,7 +10863,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A311">
         <v>4</v>
       </c>
@@ -10922,7 +10892,7 @@
         <v>41.5</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A312">
         <v>4</v>
       </c>
@@ -10951,7 +10921,7 @@
         <v>38.1</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A313">
         <v>4</v>
       </c>
@@ -10980,7 +10950,7 @@
         <v>32.1</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A314">
         <v>4</v>
       </c>
@@ -11009,7 +10979,7 @@
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A315">
         <v>4</v>
       </c>
@@ -11038,7 +11008,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A316">
         <v>4</v>
       </c>
@@ -11067,7 +11037,7 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A317">
         <v>4</v>
       </c>
@@ -11096,7 +11066,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A318">
         <v>6</v>
       </c>
@@ -11125,7 +11095,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A319">
         <v>4</v>
       </c>
@@ -11154,7 +11124,7 @@
         <v>34.299999999999997</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A320">
         <v>4</v>
       </c>
@@ -11183,7 +11153,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A321">
         <v>4</v>
       </c>
@@ -11212,7 +11182,7 @@
         <v>31.3</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A322">
         <v>4</v>
       </c>
@@ -11241,7 +11211,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A323">
         <v>4</v>
       </c>
@@ -11270,7 +11240,7 @@
         <v>32.200000000000003</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A324">
         <v>4</v>
       </c>
@@ -11299,7 +11269,7 @@
         <v>46.6</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A325">
         <v>4</v>
       </c>
@@ -11328,7 +11298,7 @@
         <v>27.9</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A326">
         <v>4</v>
       </c>
@@ -11357,7 +11327,7 @@
         <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A327">
         <v>4</v>
       </c>
@@ -11386,7 +11356,7 @@
         <v>44.3</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A328">
         <v>4</v>
       </c>
@@ -11415,7 +11385,7 @@
         <v>43.4</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A329">
         <v>5</v>
       </c>
@@ -11444,7 +11414,7 @@
         <v>36.4</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A330">
         <v>4</v>
       </c>
@@ -11473,7 +11443,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A331">
         <v>4</v>
       </c>
@@ -11502,7 +11472,7 @@
         <v>44.6</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A332">
         <v>4</v>
       </c>
@@ -11531,7 +11501,7 @@
         <v>40.9</v>
       </c>
     </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A333">
         <v>4</v>
       </c>
@@ -11560,7 +11530,7 @@
         <v>33.799999999999997</v>
       </c>
     </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A334">
         <v>4</v>
       </c>
@@ -11589,7 +11559,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A335">
         <v>6</v>
       </c>
@@ -11618,7 +11588,7 @@
         <v>32.700000000000003</v>
       </c>
     </row>
-    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A336">
         <v>3</v>
       </c>
@@ -11647,7 +11617,7 @@
         <v>23.7</v>
       </c>
     </row>
-    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A337">
         <v>4</v>
       </c>
@@ -11676,7 +11646,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A338">
         <v>4</v>
       </c>
@@ -11705,7 +11675,7 @@
         <v>23.6</v>
       </c>
     </row>
-    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A339">
         <v>4</v>
       </c>
@@ -11734,7 +11704,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A340">
         <v>4</v>
       </c>
@@ -11763,7 +11733,7 @@
         <v>27.2</v>
       </c>
     </row>
-    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A341">
         <v>4</v>
       </c>
@@ -11792,7 +11762,7 @@
         <v>26.6</v>
       </c>
     </row>
-    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A342">
         <v>4</v>
       </c>
@@ -11821,7 +11791,7 @@
         <v>25.8</v>
       </c>
     </row>
-    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A343">
         <v>6</v>
       </c>
@@ -11850,7 +11820,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A344">
         <v>4</v>
       </c>
@@ -11879,7 +11849,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A345">
         <v>4</v>
       </c>
@@ -11908,7 +11878,7 @@
         <v>39.1</v>
       </c>
     </row>
-    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A346">
         <v>4</v>
       </c>
@@ -11937,7 +11907,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A347">
         <v>4</v>
       </c>
@@ -11966,7 +11936,7 @@
         <v>35.1</v>
       </c>
     </row>
-    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A348">
         <v>4</v>
       </c>
@@ -11995,7 +11965,7 @@
         <v>32.299999999999997</v>
       </c>
     </row>
-    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A349">
         <v>4</v>
       </c>
@@ -12024,7 +11994,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A350">
         <v>4</v>
       </c>
@@ -12053,7 +12023,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="351" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A351">
         <v>4</v>
       </c>
@@ -12082,7 +12052,7 @@
         <v>34.1</v>
       </c>
     </row>
-    <row r="352" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A352">
         <v>4</v>
       </c>
@@ -12111,7 +12081,7 @@
         <v>34.700000000000003</v>
       </c>
     </row>
-    <row r="353" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A353">
         <v>4</v>
       </c>
@@ -12140,7 +12110,7 @@
         <v>34.4</v>
       </c>
     </row>
-    <row r="354" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A354">
         <v>4</v>
       </c>
@@ -12169,7 +12139,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="355" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A355">
         <v>4</v>
       </c>
@@ -12198,7 +12168,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="356" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A356">
         <v>4</v>
       </c>
@@ -12227,7 +12197,7 @@
         <v>34.5</v>
       </c>
     </row>
-    <row r="357" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A357">
         <v>4</v>
       </c>
@@ -12256,7 +12226,7 @@
         <v>33.700000000000003</v>
       </c>
     </row>
-    <row r="358" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A358">
         <v>4</v>
       </c>
@@ -12285,7 +12255,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="359" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A359">
         <v>4</v>
       </c>
@@ -12314,7 +12284,7 @@
         <v>32.9</v>
       </c>
     </row>
-    <row r="360" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A360">
         <v>4</v>
       </c>
@@ -12343,7 +12313,7 @@
         <v>31.6</v>
       </c>
     </row>
-    <row r="361" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A361">
         <v>4</v>
       </c>
@@ -12372,7 +12342,7 @@
         <v>28.1</v>
       </c>
     </row>
-    <row r="362" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A362">
         <v>6</v>
       </c>
@@ -12401,7 +12371,7 @@
         <v>30.7</v>
       </c>
     </row>
-    <row r="363" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A363">
         <v>6</v>
       </c>
@@ -12430,7 +12400,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="364" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A364">
         <v>6</v>
       </c>
@@ -12459,7 +12429,7 @@
         <v>24.2</v>
       </c>
     </row>
-    <row r="365" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A365">
         <v>6</v>
       </c>
@@ -12488,7 +12458,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="366" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A366">
         <v>8</v>
       </c>
@@ -12517,7 +12487,7 @@
         <v>26.6</v>
       </c>
     </row>
-    <row r="367" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A367">
         <v>6</v>
       </c>
@@ -12546,7 +12516,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="368" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A368">
         <v>6</v>
       </c>
@@ -12575,7 +12545,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="369" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A369">
         <v>4</v>
       </c>
@@ -12604,7 +12574,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="370" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A370">
         <v>4</v>
       </c>
@@ -12633,7 +12603,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="371" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A371">
         <v>4</v>
       </c>
@@ -12662,7 +12632,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="372" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A372">
         <v>4</v>
       </c>
@@ -12691,7 +12661,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="373" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A373">
         <v>4</v>
       </c>
@@ -12720,7 +12690,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="374" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A374">
         <v>4</v>
       </c>
@@ -12749,7 +12719,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="375" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A375">
         <v>4</v>
       </c>
@@ -12778,7 +12748,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="376" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A376">
         <v>4</v>
       </c>
@@ -12807,7 +12777,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="377" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A377">
         <v>4</v>
       </c>
@@ -12836,7 +12806,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="378" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A378">
         <v>4</v>
       </c>
@@ -12865,7 +12835,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="379" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A379">
         <v>4</v>
       </c>
@@ -12894,7 +12864,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="380" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A380">
         <v>4</v>
       </c>
@@ -12923,7 +12893,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="381" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A381">
         <v>4</v>
       </c>
@@ -12952,7 +12922,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="382" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A382">
         <v>4</v>
       </c>
@@ -12981,7 +12951,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="383" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A383">
         <v>4</v>
       </c>
@@ -13010,7 +12980,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="384" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A384">
         <v>4</v>
       </c>
@@ -13039,7 +13009,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="385" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A385">
         <v>4</v>
       </c>
@@ -13068,7 +13038,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="386" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A386">
         <v>4</v>
       </c>
@@ -13097,7 +13067,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="387" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A387">
         <v>4</v>
       </c>
@@ -13126,7 +13096,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="388" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A388">
         <v>6</v>
       </c>
@@ -13155,7 +13125,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="389" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A389">
         <v>6</v>
       </c>
@@ -13184,7 +13154,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="390" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A390">
         <v>4</v>
       </c>
@@ -13213,7 +13183,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="391" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A391">
         <v>6</v>
       </c>
@@ -13242,7 +13212,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="392" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A392">
         <v>4</v>
       </c>
@@ -13271,7 +13241,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="393" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A393">
         <v>4</v>
       </c>
@@ -13300,7 +13270,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="394" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A394">
         <v>4</v>
       </c>
@@ -13329,7 +13299,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="395" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A395">
         <v>4</v>
       </c>
@@ -13358,7 +13328,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="396" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A396">
         <v>4</v>
       </c>
@@ -13387,7 +13357,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="397" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A397">
         <v>4</v>
       </c>
@@ -13416,7 +13386,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="398" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A398">
         <v>4</v>
       </c>
@@ -13445,7 +13415,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="399" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A399">
         <v>4</v>
       </c>
@@ -13472,267 +13442,6 @@
       </c>
       <c r="I399">
         <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>17</v>
-      </c>
-      <c r="D3">
-        <f>B3-C3</f>
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <f>D3*D3</f>
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <f>$B$10</f>
-        <v>18.333333333333332</v>
-      </c>
-      <c r="G3">
-        <f>B3-F3</f>
-        <v>-0.33333333333333215</v>
-      </c>
-      <c r="H3">
-        <f>G3*G3</f>
-        <v>0.11111111111111033</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D8" si="0">B4-C4</f>
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E8" si="1">D4*D4</f>
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F8" si="2">$B$10</f>
-        <v>18.333333333333332</v>
-      </c>
-      <c r="G4">
-        <f t="shared" ref="G4:G8" si="3">B4-F4</f>
-        <v>-3.3333333333333321</v>
-      </c>
-      <c r="H4">
-        <f t="shared" ref="H4:H8" si="4">G4*G4</f>
-        <v>11.111111111111104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>25</v>
-      </c>
-      <c r="C5">
-        <v>23</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="2"/>
-        <v>18.333333333333332</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="3"/>
-        <v>6.6666666666666679</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="4"/>
-        <v>44.444444444444457</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="2"/>
-        <v>18.333333333333332</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="3"/>
-        <v>-2.3333333333333321</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="4"/>
-        <v>5.4444444444444393</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>21</v>
-      </c>
-      <c r="C7">
-        <v>19</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="2"/>
-        <v>18.333333333333332</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="3"/>
-        <v>2.6666666666666679</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="4"/>
-        <v>7.1111111111111178</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>14</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="2"/>
-        <v>18.333333333333332</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="3"/>
-        <v>-3.3333333333333321</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="4"/>
-        <v>11.111111111111104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>320</v>
-      </c>
-      <c r="B10">
-        <f>AVERAGE(B3:B8)</f>
-        <v>18.333333333333332</v>
-      </c>
-      <c r="D10" t="s">
-        <v>317</v>
-      </c>
-      <c r="E10">
-        <f>SUM(E3:E8)</f>
-        <v>14</v>
-      </c>
-      <c r="G10" t="s">
-        <v>316</v>
-      </c>
-      <c r="H10">
-        <f>SUM(H3:H8)</f>
-        <v>79.333333333333329</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>324</v>
-      </c>
-      <c r="D12">
-        <f>1-(E10/H10)</f>
-        <v>0.82352941176470584</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>